<commit_message>
neaten up UI and message panels
</commit_message>
<xml_diff>
--- a/roguelike/model/data/rogue_stats.xlsx
+++ b/roguelike/model/data/rogue_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Development\Python\roguelike\roguelike\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80287224-4A12-4EDC-AAF5-CC97125ACB1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53FE125-D082-420C-9C87-35D04B549FD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="2220" windowWidth="24855" windowHeight="17160" tabRatio="800" firstSheet="7" activeTab="16" xr2:uid="{5CB7D2FB-DC00-41F8-A371-36122BC790D1}"/>
+    <workbookView xWindow="8655" yWindow="1140" windowWidth="24855" windowHeight="17160" tabRatio="800" firstSheet="7" activeTab="16" xr2:uid="{5CB7D2FB-DC00-41F8-A371-36122BC790D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -41658,7 +41658,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L20"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
tidy up some entity stats
</commit_message>
<xml_diff>
--- a/roguelike/model/data/rogue_stats.xlsx
+++ b/roguelike/model/data/rogue_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Development\Python\roguelike\roguelike\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA9B2F1-6C0C-4CD0-BD83-35044C69050F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B22D13-4A30-4713-AA34-04591FB4D32E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="1755" windowWidth="27720" windowHeight="18690" tabRatio="671" firstSheet="9" activeTab="18" xr2:uid="{5CB7D2FB-DC00-41F8-A371-36122BC790D1}"/>
+    <workbookView xWindow="5340" yWindow="1245" windowWidth="27720" windowHeight="18690" tabRatio="671" firstSheet="9" activeTab="18" xr2:uid="{5CB7D2FB-DC00-41F8-A371-36122BC790D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -147,20 +147,20 @@
     <t>Scope</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>Probability</t>
   </si>
   <si>
-    <t>Room</t>
+    <t>Plate Armour</t>
   </si>
   <si>
-    <t>Orc</t>
+    <t>Floor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,8 +176,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +224,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -537,6 +550,24 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -10803,157 +10834,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.6999999999999997</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.3</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.9000000000000004</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.2</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.5</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.8</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.1</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.3999999999999995</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.7</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.3</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.6</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.8999999999999995</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.1999999999999993</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.5</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8.8000000000000007</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9.1</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9.4</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>9.6999999999999993</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>10.299999999999999</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>10.6</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>10.9</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>11.2</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>11.5</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>11.799999999999999</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>12.1</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>12.4</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>12.7</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>13</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>13.299999999999999</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>13.6</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>13.9</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>14.2</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>14.5</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>14.799999999999999</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>15.1</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>15.399999999999999</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>15.7</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>16</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11220,97 +11251,97 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-20</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-40</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11517,157 +11548,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -47734,7 +47765,7 @@
   <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="L5" sqref="L5:U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47755,31 +47786,31 @@
       <c r="A1" s="17">
         <v>1</v>
       </c>
-      <c r="B1" s="19">
+      <c r="B1" s="36">
         <f>P5</f>
-        <v>0.3</v>
-      </c>
-      <c r="C1" s="20">
+        <v>2</v>
+      </c>
+      <c r="C1" s="37">
         <f>Q5</f>
-        <v>1</v>
-      </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="28">
+        <v>0</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39">
         <f>R5</f>
         <v>20</v>
       </c>
-      <c r="F1" s="20">
+      <c r="F1" s="37">
         <f>S5</f>
-        <v>-20</v>
-      </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="16">
+        <v>-100</v>
+      </c>
+      <c r="G1" s="40"/>
+      <c r="H1" s="41">
         <f>T5</f>
-        <v>0</v>
-      </c>
-      <c r="I1" s="16">
+        <v>10</v>
+      </c>
+      <c r="I1" s="41">
         <f>U5</f>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J1" s="14"/>
       <c r="M1" s="31" t="s">
@@ -47839,11 +47870,11 @@
       </c>
       <c r="M2" s="30">
         <f>B1</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="N2" s="30">
         <f>C1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2" s="30">
         <f>E1</f>
@@ -47851,15 +47882,15 @@
       </c>
       <c r="P2" s="30">
         <f>F1</f>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="Q2" s="30">
         <f>H1</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R2" s="30">
         <f>I1</f>
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -47872,11 +47903,11 @@
       </c>
       <c r="C3" s="2">
         <f>C$1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="25">
         <f>SUM(B3:C3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="29">
         <f t="shared" ref="E3:E40" si="0">QUOTIENT(A3,$E$1)</f>
@@ -47888,19 +47919,19 @@
       </c>
       <c r="G3" s="4">
         <f>D3+F3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="5">
         <f>H$1</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I3" s="5">
         <f>I$1</f>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J3" s="15">
         <f>MIN(MAX(H3,INT(G3)),I3)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -47910,15 +47941,15 @@
       </c>
       <c r="B4" s="24">
         <f t="shared" ref="B4:B40" si="1">$B$1*A4</f>
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:C53" si="2">C$1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="25">
         <f t="shared" ref="D4:D40" si="3">SUM(B4:C4)</f>
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="29">
         <f t="shared" si="0"/>
@@ -47930,19 +47961,19 @@
       </c>
       <c r="G4" s="4">
         <f t="shared" ref="G4:G40" si="5">D4+F4</f>
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" ref="H4:I41" si="6">H$1</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J4" s="15">
         <f t="shared" ref="J4:J40" si="7">MIN(MAX(H4,INT(G4)),I4)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L4" s="35" t="s">
         <v>29</v>
@@ -47982,15 +48013,15 @@
       </c>
       <c r="B5" s="24">
         <f t="shared" si="1"/>
-        <v>0.6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="25">
         <f t="shared" si="3"/>
-        <v>1.6</v>
+        <v>4</v>
       </c>
       <c r="E5" s="29">
         <f t="shared" si="0"/>
@@ -48002,49 +48033,49 @@
       </c>
       <c r="G5" s="4">
         <f t="shared" si="5"/>
-        <v>1.6</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J5" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M5" t="s">
         <v>32</v>
       </c>
       <c r="N5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O5" t="s">
         <v>20</v>
       </c>
       <c r="P5">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <v>20</v>
       </c>
       <c r="S5">
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U5">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -48054,15 +48085,15 @@
       </c>
       <c r="B6" s="24">
         <f t="shared" si="1"/>
-        <v>0.89999999999999991</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="25">
         <f t="shared" si="3"/>
-        <v>1.9</v>
+        <v>6</v>
       </c>
       <c r="E6" s="29">
         <f t="shared" si="0"/>
@@ -48074,19 +48105,19 @@
       </c>
       <c r="G6" s="4">
         <f t="shared" si="5"/>
-        <v>1.9</v>
+        <v>6</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J6" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -48096,15 +48127,15 @@
       </c>
       <c r="B7" s="24">
         <f t="shared" si="1"/>
-        <v>1.2</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="25">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>8</v>
       </c>
       <c r="E7" s="29">
         <f t="shared" si="0"/>
@@ -48116,19 +48147,19 @@
       </c>
       <c r="G7" s="4">
         <f t="shared" si="5"/>
-        <v>2.2000000000000002</v>
+        <v>8</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J7" s="15">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -48138,15 +48169,15 @@
       </c>
       <c r="B8" s="24">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="25">
         <f t="shared" si="3"/>
-        <v>2.5</v>
+        <v>10</v>
       </c>
       <c r="E8" s="29">
         <f t="shared" si="0"/>
@@ -48158,19 +48189,19 @@
       </c>
       <c r="G8" s="4">
         <f t="shared" si="5"/>
-        <v>2.5</v>
+        <v>10</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J8" s="15">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -48180,15 +48211,15 @@
       </c>
       <c r="B9" s="24">
         <f t="shared" si="1"/>
-        <v>1.7999999999999998</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="25">
         <f t="shared" si="3"/>
-        <v>2.8</v>
+        <v>12</v>
       </c>
       <c r="E9" s="29">
         <f t="shared" si="0"/>
@@ -48200,19 +48231,19 @@
       </c>
       <c r="G9" s="4">
         <f t="shared" si="5"/>
-        <v>2.8</v>
+        <v>12</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J9" s="15">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -48222,15 +48253,15 @@
       </c>
       <c r="B10" s="24">
         <f t="shared" si="1"/>
-        <v>2.1</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="25">
         <f t="shared" si="3"/>
-        <v>3.1</v>
+        <v>14</v>
       </c>
       <c r="E10" s="29">
         <f t="shared" si="0"/>
@@ -48242,19 +48273,19 @@
       </c>
       <c r="G10" s="4">
         <f t="shared" si="5"/>
-        <v>3.1</v>
+        <v>14</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J10" s="15">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -48264,15 +48295,15 @@
       </c>
       <c r="B11" s="24">
         <f t="shared" si="1"/>
-        <v>2.4</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="25">
         <f t="shared" si="3"/>
-        <v>3.4</v>
+        <v>16</v>
       </c>
       <c r="E11" s="29">
         <f t="shared" si="0"/>
@@ -48284,19 +48315,19 @@
       </c>
       <c r="G11" s="4">
         <f t="shared" si="5"/>
-        <v>3.4</v>
+        <v>16</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J11" s="15">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -48306,15 +48337,15 @@
       </c>
       <c r="B12" s="24">
         <f t="shared" si="1"/>
-        <v>2.6999999999999997</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="25">
         <f t="shared" si="3"/>
-        <v>3.6999999999999997</v>
+        <v>18</v>
       </c>
       <c r="E12" s="29">
         <f t="shared" si="0"/>
@@ -48326,19 +48357,19 @@
       </c>
       <c r="G12" s="4">
         <f t="shared" si="5"/>
-        <v>3.6999999999999997</v>
+        <v>18</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J12" s="15">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -48348,15 +48379,15 @@
       </c>
       <c r="B13" s="24">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="25">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E13" s="29">
         <f t="shared" si="0"/>
@@ -48368,19 +48399,19 @@
       </c>
       <c r="G13" s="4">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J13" s="15">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -48390,15 +48421,15 @@
       </c>
       <c r="B14" s="24">
         <f t="shared" si="1"/>
-        <v>3.3</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="25">
         <f t="shared" si="3"/>
-        <v>4.3</v>
+        <v>22</v>
       </c>
       <c r="E14" s="29">
         <f t="shared" si="0"/>
@@ -48410,19 +48441,19 @@
       </c>
       <c r="G14" s="4">
         <f t="shared" si="5"/>
-        <v>4.3</v>
+        <v>22</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J14" s="15">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -48432,15 +48463,15 @@
       </c>
       <c r="B15" s="24">
         <f t="shared" si="1"/>
-        <v>3.5999999999999996</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="25">
         <f t="shared" si="3"/>
-        <v>4.5999999999999996</v>
+        <v>24</v>
       </c>
       <c r="E15" s="29">
         <f t="shared" si="0"/>
@@ -48452,19 +48483,19 @@
       </c>
       <c r="G15" s="4">
         <f t="shared" si="5"/>
-        <v>4.5999999999999996</v>
+        <v>24</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J15" s="15">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -48474,15 +48505,15 @@
       </c>
       <c r="B16" s="24">
         <f t="shared" si="1"/>
-        <v>3.9</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="25">
         <f t="shared" si="3"/>
-        <v>4.9000000000000004</v>
+        <v>26</v>
       </c>
       <c r="E16" s="29">
         <f t="shared" si="0"/>
@@ -48494,19 +48525,19 @@
       </c>
       <c r="G16" s="4">
         <f t="shared" si="5"/>
-        <v>4.9000000000000004</v>
+        <v>26</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J16" s="15">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -48516,15 +48547,15 @@
       </c>
       <c r="B17" s="24">
         <f t="shared" si="1"/>
-        <v>4.2</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="25">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>28</v>
       </c>
       <c r="E17" s="29">
         <f t="shared" si="0"/>
@@ -48536,19 +48567,19 @@
       </c>
       <c r="G17" s="4">
         <f t="shared" si="5"/>
-        <v>5.2</v>
+        <v>28</v>
       </c>
       <c r="H17" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J17" s="15">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -48558,15 +48589,15 @@
       </c>
       <c r="B18" s="24">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="25">
         <f t="shared" si="3"/>
-        <v>5.5</v>
+        <v>30</v>
       </c>
       <c r="E18" s="29">
         <f t="shared" si="0"/>
@@ -48578,19 +48609,19 @@
       </c>
       <c r="G18" s="4">
         <f t="shared" si="5"/>
-        <v>5.5</v>
+        <v>30</v>
       </c>
       <c r="H18" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J18" s="15">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -48600,15 +48631,15 @@
       </c>
       <c r="B19" s="24">
         <f t="shared" si="1"/>
-        <v>4.8</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="25">
         <f t="shared" si="3"/>
-        <v>5.8</v>
+        <v>32</v>
       </c>
       <c r="E19" s="29">
         <f t="shared" si="0"/>
@@ -48620,19 +48651,19 @@
       </c>
       <c r="G19" s="4">
         <f t="shared" si="5"/>
-        <v>5.8</v>
+        <v>32</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I19" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J19" s="15">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -48642,15 +48673,15 @@
       </c>
       <c r="B20" s="24">
         <f t="shared" si="1"/>
-        <v>5.0999999999999996</v>
+        <v>34</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="25">
         <f t="shared" si="3"/>
-        <v>6.1</v>
+        <v>34</v>
       </c>
       <c r="E20" s="29">
         <f t="shared" si="0"/>
@@ -48662,19 +48693,19 @@
       </c>
       <c r="G20" s="4">
         <f t="shared" si="5"/>
-        <v>6.1</v>
+        <v>34</v>
       </c>
       <c r="H20" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I20" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J20" s="15">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -48684,15 +48715,15 @@
       </c>
       <c r="B21" s="24">
         <f t="shared" si="1"/>
-        <v>5.3999999999999995</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="25">
         <f t="shared" si="3"/>
-        <v>6.3999999999999995</v>
+        <v>36</v>
       </c>
       <c r="E21" s="29">
         <f t="shared" si="0"/>
@@ -48704,19 +48735,19 @@
       </c>
       <c r="G21" s="4">
         <f t="shared" si="5"/>
-        <v>6.3999999999999995</v>
+        <v>36</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I21" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J21" s="15">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -48726,15 +48757,15 @@
       </c>
       <c r="B22" s="24">
         <f t="shared" si="1"/>
-        <v>5.7</v>
+        <v>38</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="25">
         <f t="shared" si="3"/>
-        <v>6.7</v>
+        <v>38</v>
       </c>
       <c r="E22" s="29">
         <f t="shared" si="0"/>
@@ -48746,19 +48777,19 @@
       </c>
       <c r="G22" s="4">
         <f t="shared" si="5"/>
-        <v>6.7</v>
+        <v>38</v>
       </c>
       <c r="H22" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I22" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J22" s="15">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -48768,39 +48799,39 @@
       </c>
       <c r="B23" s="24">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="25">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="E23" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D23" s="25">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="E23" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F23" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="5"/>
-        <v>-13</v>
+        <v>-60</v>
       </c>
       <c r="H23" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I23" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J23" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -48810,39 +48841,39 @@
       </c>
       <c r="B24" s="24">
         <f t="shared" si="1"/>
-        <v>6.3</v>
+        <v>42</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="25">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="E24" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D24" s="25">
-        <f t="shared" si="3"/>
-        <v>7.3</v>
-      </c>
-      <c r="E24" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F24" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="5"/>
-        <v>-12.7</v>
+        <v>-58</v>
       </c>
       <c r="H24" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I24" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J24" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -48852,39 +48883,39 @@
       </c>
       <c r="B25" s="24">
         <f t="shared" si="1"/>
-        <v>6.6</v>
+        <v>44</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="25">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="E25" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D25" s="25">
-        <f t="shared" si="3"/>
-        <v>7.6</v>
-      </c>
-      <c r="E25" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F25" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="5"/>
-        <v>-12.4</v>
+        <v>-56</v>
       </c>
       <c r="H25" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I25" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J25" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -48894,39 +48925,39 @@
       </c>
       <c r="B26" s="24">
         <f t="shared" si="1"/>
-        <v>6.8999999999999995</v>
+        <v>46</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="25">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="E26" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D26" s="25">
-        <f t="shared" si="3"/>
-        <v>7.8999999999999995</v>
-      </c>
-      <c r="E26" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F26" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="5"/>
-        <v>-12.100000000000001</v>
+        <v>-54</v>
       </c>
       <c r="H26" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I26" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J26" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -48936,39 +48967,39 @@
       </c>
       <c r="B27" s="24">
         <f t="shared" si="1"/>
-        <v>7.1999999999999993</v>
+        <v>48</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="25">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="E27" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D27" s="25">
-        <f t="shared" si="3"/>
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="E27" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F27" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="5"/>
-        <v>-11.8</v>
+        <v>-52</v>
       </c>
       <c r="H27" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I27" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J27" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -48978,39 +49009,39 @@
       </c>
       <c r="B28" s="24">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>50</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="25">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="E28" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D28" s="25">
-        <f t="shared" si="3"/>
-        <v>8.5</v>
-      </c>
-      <c r="E28" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F28" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="5"/>
-        <v>-11.5</v>
+        <v>-50</v>
       </c>
       <c r="H28" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I28" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J28" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -49020,39 +49051,39 @@
       </c>
       <c r="B29" s="24">
         <f t="shared" si="1"/>
-        <v>7.8</v>
+        <v>52</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D29" s="25">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="E29" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D29" s="25">
-        <f t="shared" si="3"/>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E29" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F29" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="5"/>
-        <v>-11.2</v>
+        <v>-48</v>
       </c>
       <c r="H29" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I29" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J29" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -49062,39 +49093,39 @@
       </c>
       <c r="B30" s="24">
         <f t="shared" si="1"/>
-        <v>8.1</v>
+        <v>54</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="25">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="E30" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D30" s="25">
-        <f t="shared" si="3"/>
-        <v>9.1</v>
-      </c>
-      <c r="E30" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F30" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="5"/>
-        <v>-10.9</v>
+        <v>-46</v>
       </c>
       <c r="H30" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I30" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J30" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -49104,39 +49135,39 @@
       </c>
       <c r="B31" s="24">
         <f t="shared" si="1"/>
-        <v>8.4</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="25">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="E31" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D31" s="25">
-        <f t="shared" si="3"/>
-        <v>9.4</v>
-      </c>
-      <c r="E31" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F31" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="5"/>
-        <v>-10.6</v>
+        <v>-44</v>
       </c>
       <c r="H31" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I31" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J31" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -49146,39 +49177,39 @@
       </c>
       <c r="B32" s="24">
         <f t="shared" si="1"/>
-        <v>8.6999999999999993</v>
+        <v>58</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="25">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="E32" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D32" s="25">
-        <f t="shared" si="3"/>
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="E32" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F32" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G32" s="4">
         <f t="shared" si="5"/>
-        <v>-10.3</v>
+        <v>-42</v>
       </c>
       <c r="H32" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I32" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J32" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -49188,39 +49219,39 @@
       </c>
       <c r="B33" s="24">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C33" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="25">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="E33" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D33" s="25">
-        <f t="shared" si="3"/>
+      <c r="F33" s="3">
+        <f t="shared" si="4"/>
+        <v>-100</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="5"/>
+        <v>-40</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="E33" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F33" s="3">
-        <f t="shared" si="4"/>
-        <v>-20</v>
-      </c>
-      <c r="G33" s="4">
-        <f t="shared" si="5"/>
-        <v>-10</v>
-      </c>
-      <c r="H33" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="I33" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J33" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -49230,39 +49261,39 @@
       </c>
       <c r="B34" s="24">
         <f t="shared" si="1"/>
-        <v>9.2999999999999989</v>
+        <v>62</v>
       </c>
       <c r="C34" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="25">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="E34" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D34" s="25">
-        <f t="shared" si="3"/>
-        <v>10.299999999999999</v>
-      </c>
-      <c r="E34" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F34" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G34" s="4">
         <f t="shared" si="5"/>
-        <v>-9.7000000000000011</v>
+        <v>-38</v>
       </c>
       <c r="H34" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I34" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J34" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -49272,39 +49303,39 @@
       </c>
       <c r="B35" s="24">
         <f t="shared" si="1"/>
-        <v>9.6</v>
+        <v>64</v>
       </c>
       <c r="C35" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D35" s="25">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="E35" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D35" s="25">
-        <f t="shared" si="3"/>
-        <v>10.6</v>
-      </c>
-      <c r="E35" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F35" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="5"/>
-        <v>-9.4</v>
+        <v>-36</v>
       </c>
       <c r="H35" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I35" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J35" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -49314,39 +49345,39 @@
       </c>
       <c r="B36" s="24">
         <f t="shared" si="1"/>
-        <v>9.9</v>
+        <v>66</v>
       </c>
       <c r="C36" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="25">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="E36" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D36" s="25">
-        <f t="shared" si="3"/>
-        <v>10.9</v>
-      </c>
-      <c r="E36" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F36" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G36" s="4">
         <f t="shared" si="5"/>
-        <v>-9.1</v>
+        <v>-34</v>
       </c>
       <c r="H36" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I36" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J36" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -49356,39 +49387,39 @@
       </c>
       <c r="B37" s="24">
         <f t="shared" si="1"/>
-        <v>10.199999999999999</v>
+        <v>68</v>
       </c>
       <c r="C37" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="25">
+        <f t="shared" si="3"/>
+        <v>68</v>
+      </c>
+      <c r="E37" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D37" s="25">
-        <f t="shared" si="3"/>
-        <v>11.2</v>
-      </c>
-      <c r="E37" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F37" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G37" s="4">
         <f t="shared" si="5"/>
-        <v>-8.8000000000000007</v>
+        <v>-32</v>
       </c>
       <c r="H37" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I37" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J37" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -49398,39 +49429,39 @@
       </c>
       <c r="B38" s="24">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>70</v>
       </c>
       <c r="C38" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="25">
+        <f t="shared" si="3"/>
+        <v>70</v>
+      </c>
+      <c r="E38" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D38" s="25">
-        <f t="shared" si="3"/>
-        <v>11.5</v>
-      </c>
-      <c r="E38" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F38" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G38" s="4">
         <f t="shared" si="5"/>
-        <v>-8.5</v>
+        <v>-30</v>
       </c>
       <c r="H38" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I38" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J38" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -49440,39 +49471,39 @@
       </c>
       <c r="B39" s="24">
         <f t="shared" si="1"/>
-        <v>10.799999999999999</v>
+        <v>72</v>
       </c>
       <c r="C39" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="25">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+      <c r="E39" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D39" s="25">
-        <f t="shared" si="3"/>
-        <v>11.799999999999999</v>
-      </c>
-      <c r="E39" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F39" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="5"/>
-        <v>-8.2000000000000011</v>
+        <v>-28</v>
       </c>
       <c r="H39" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I39" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J39" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -49482,39 +49513,39 @@
       </c>
       <c r="B40" s="24">
         <f t="shared" si="1"/>
-        <v>11.1</v>
+        <v>74</v>
       </c>
       <c r="C40" s="2">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="25">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+      <c r="E40" s="29">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="D40" s="25">
-        <f t="shared" si="3"/>
-        <v>12.1</v>
-      </c>
-      <c r="E40" s="29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="F40" s="3">
         <f t="shared" si="4"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="5"/>
-        <v>-7.9</v>
+        <v>-26</v>
       </c>
       <c r="H40" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I40" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J40" s="15">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -49524,15 +49555,15 @@
       </c>
       <c r="B41" s="24">
         <f t="shared" ref="B41:B53" si="10">$B$1*A41</f>
-        <v>11.4</v>
+        <v>76</v>
       </c>
       <c r="C41" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="25">
         <f t="shared" ref="D41:D53" si="11">SUM(B41:C41)</f>
-        <v>12.4</v>
+        <v>76</v>
       </c>
       <c r="E41" s="29">
         <f t="shared" ref="E41:E53" si="12">QUOTIENT(A41,$E$1)</f>
@@ -49540,23 +49571,23 @@
       </c>
       <c r="F41" s="3">
         <f t="shared" ref="F41:F53" si="13">E41*F$1</f>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" ref="G41:G53" si="14">D41+F41</f>
-        <v>-7.6</v>
+        <v>-24</v>
       </c>
       <c r="H41" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I41" s="5">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J41" s="15">
         <f t="shared" ref="J41:J53" si="15">MIN(MAX(H41,INT(G41)),I41)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -49566,15 +49597,15 @@
       </c>
       <c r="B42" s="24">
         <f t="shared" si="10"/>
-        <v>11.7</v>
+        <v>78</v>
       </c>
       <c r="C42" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" s="25">
         <f t="shared" si="11"/>
-        <v>12.7</v>
+        <v>78</v>
       </c>
       <c r="E42" s="29">
         <f t="shared" si="12"/>
@@ -49582,23 +49613,23 @@
       </c>
       <c r="F42" s="3">
         <f t="shared" si="13"/>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="14"/>
-        <v>-7.3000000000000007</v>
+        <v>-22</v>
       </c>
       <c r="H42" s="5">
         <f t="shared" ref="H42:I53" si="16">H$1</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I42" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J42" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -49608,15 +49639,15 @@
       </c>
       <c r="B43" s="24">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="C43" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" s="25">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="E43" s="29">
         <f t="shared" si="12"/>
@@ -49624,23 +49655,23 @@
       </c>
       <c r="F43" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G43" s="4">
         <f t="shared" si="14"/>
-        <v>-27</v>
+        <v>-120</v>
       </c>
       <c r="H43" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I43" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J43" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -49650,15 +49681,15 @@
       </c>
       <c r="B44" s="24">
         <f t="shared" si="10"/>
-        <v>12.299999999999999</v>
+        <v>82</v>
       </c>
       <c r="C44" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="25">
         <f t="shared" si="11"/>
-        <v>13.299999999999999</v>
+        <v>82</v>
       </c>
       <c r="E44" s="29">
         <f t="shared" si="12"/>
@@ -49666,23 +49697,23 @@
       </c>
       <c r="F44" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G44" s="4">
         <f t="shared" si="14"/>
-        <v>-26.700000000000003</v>
+        <v>-118</v>
       </c>
       <c r="H44" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I44" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J44" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -49692,15 +49723,15 @@
       </c>
       <c r="B45" s="24">
         <f t="shared" si="10"/>
-        <v>12.6</v>
+        <v>84</v>
       </c>
       <c r="C45" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="25">
         <f t="shared" si="11"/>
-        <v>13.6</v>
+        <v>84</v>
       </c>
       <c r="E45" s="29">
         <f t="shared" si="12"/>
@@ -49708,23 +49739,23 @@
       </c>
       <c r="F45" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G45" s="4">
         <f t="shared" si="14"/>
-        <v>-26.4</v>
+        <v>-116</v>
       </c>
       <c r="H45" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I45" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J45" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -49734,15 +49765,15 @@
       </c>
       <c r="B46" s="24">
         <f t="shared" si="10"/>
-        <v>12.9</v>
+        <v>86</v>
       </c>
       <c r="C46" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="25">
         <f t="shared" si="11"/>
-        <v>13.9</v>
+        <v>86</v>
       </c>
       <c r="E46" s="29">
         <f t="shared" si="12"/>
@@ -49750,23 +49781,23 @@
       </c>
       <c r="F46" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G46" s="4">
         <f t="shared" si="14"/>
-        <v>-26.1</v>
+        <v>-114</v>
       </c>
       <c r="H46" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I46" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J46" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -49776,15 +49807,15 @@
       </c>
       <c r="B47" s="24">
         <f t="shared" si="10"/>
-        <v>13.2</v>
+        <v>88</v>
       </c>
       <c r="C47" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" s="25">
         <f t="shared" si="11"/>
-        <v>14.2</v>
+        <v>88</v>
       </c>
       <c r="E47" s="29">
         <f t="shared" si="12"/>
@@ -49792,23 +49823,23 @@
       </c>
       <c r="F47" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G47" s="4">
         <f t="shared" si="14"/>
-        <v>-25.8</v>
+        <v>-112</v>
       </c>
       <c r="H47" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I47" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J47" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -49818,15 +49849,15 @@
       </c>
       <c r="B48" s="24">
         <f t="shared" si="10"/>
-        <v>13.5</v>
+        <v>90</v>
       </c>
       <c r="C48" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="25">
         <f t="shared" si="11"/>
-        <v>14.5</v>
+        <v>90</v>
       </c>
       <c r="E48" s="29">
         <f t="shared" si="12"/>
@@ -49834,23 +49865,23 @@
       </c>
       <c r="F48" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G48" s="4">
         <f t="shared" si="14"/>
-        <v>-25.5</v>
+        <v>-110</v>
       </c>
       <c r="H48" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I48" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J48" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -49860,15 +49891,15 @@
       </c>
       <c r="B49" s="24">
         <f t="shared" si="10"/>
-        <v>13.799999999999999</v>
+        <v>92</v>
       </c>
       <c r="C49" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" s="25">
         <f t="shared" si="11"/>
-        <v>14.799999999999999</v>
+        <v>92</v>
       </c>
       <c r="E49" s="29">
         <f t="shared" si="12"/>
@@ -49876,23 +49907,23 @@
       </c>
       <c r="F49" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G49" s="4">
         <f t="shared" si="14"/>
-        <v>-25.200000000000003</v>
+        <v>-108</v>
       </c>
       <c r="H49" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I49" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J49" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -49902,15 +49933,15 @@
       </c>
       <c r="B50" s="24">
         <f t="shared" si="10"/>
-        <v>14.1</v>
+        <v>94</v>
       </c>
       <c r="C50" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" s="25">
         <f t="shared" si="11"/>
-        <v>15.1</v>
+        <v>94</v>
       </c>
       <c r="E50" s="29">
         <f t="shared" si="12"/>
@@ -49918,23 +49949,23 @@
       </c>
       <c r="F50" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G50" s="4">
         <f t="shared" si="14"/>
-        <v>-24.9</v>
+        <v>-106</v>
       </c>
       <c r="H50" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I50" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J50" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -49944,15 +49975,15 @@
       </c>
       <c r="B51" s="24">
         <f t="shared" si="10"/>
-        <v>14.399999999999999</v>
+        <v>96</v>
       </c>
       <c r="C51" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" s="25">
         <f t="shared" si="11"/>
-        <v>15.399999999999999</v>
+        <v>96</v>
       </c>
       <c r="E51" s="29">
         <f t="shared" si="12"/>
@@ -49960,23 +49991,23 @@
       </c>
       <c r="F51" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G51" s="4">
         <f t="shared" si="14"/>
-        <v>-24.6</v>
+        <v>-104</v>
       </c>
       <c r="H51" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I51" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J51" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -49986,15 +50017,15 @@
       </c>
       <c r="B52" s="24">
         <f t="shared" si="10"/>
-        <v>14.7</v>
+        <v>98</v>
       </c>
       <c r="C52" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" s="25">
         <f t="shared" si="11"/>
-        <v>15.7</v>
+        <v>98</v>
       </c>
       <c r="E52" s="29">
         <f t="shared" si="12"/>
@@ -50002,23 +50033,23 @@
       </c>
       <c r="F52" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G52" s="4">
         <f t="shared" si="14"/>
-        <v>-24.3</v>
+        <v>-102</v>
       </c>
       <c r="H52" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I52" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J52" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -50028,15 +50059,15 @@
       </c>
       <c r="B53" s="24">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="C53" s="2">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="25">
         <f t="shared" si="11"/>
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="E53" s="29">
         <f t="shared" si="12"/>
@@ -50044,23 +50075,23 @@
       </c>
       <c r="F53" s="3">
         <f t="shared" si="13"/>
-        <v>-40</v>
+        <v>-200</v>
       </c>
       <c r="G53" s="4">
         <f t="shared" si="14"/>
-        <v>-24</v>
+        <v>-100</v>
       </c>
       <c r="H53" s="5">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I53" s="5">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="J53" s="15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shop tidy up more weapons added
</commit_message>
<xml_diff>
--- a/roguelike/model/data/rogue_stats.xlsx
+++ b/roguelike/model/data/rogue_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Development\Python\roguelike\roguelike\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C477D7E-9072-4B0A-A723-E0514999DDCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7245BC8-0145-4DDA-A6FF-3F1934D70441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="671" firstSheet="9" activeTab="19" xr2:uid="{5CB7D2FB-DC00-41F8-A371-36122BC790D1}"/>
   </bookViews>
@@ -13351,157 +13351,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>-16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-13</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="21">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="27">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="33">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="39">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>30.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>31.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="45">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>101</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>104</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>107</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>119</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13522,7 +13522,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ax5</c:v>
+                  <c:v>ax10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -13723,19 +13723,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
@@ -13753,19 +13753,19 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>2</c:v>
@@ -13783,19 +13783,19 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>3</c:v>
@@ -13813,19 +13813,19 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>4</c:v>
@@ -13843,19 +13843,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>5</c:v>
@@ -14071,151 +14071,151 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="35">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>50</c:v>
-                </c:pt>
                 <c:pt idx="45">
-                  <c:v>50</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>50</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>50</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>50</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>50</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>50</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -53882,7 +53882,7 @@
   <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="L5" sqref="L5:U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53906,20 +53906,20 @@
       </c>
       <c r="B1" s="36">
         <f>P5</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="C1" s="37">
         <f>Q5</f>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D1" s="38"/>
       <c r="E1" s="39">
         <f>R5</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F1" s="37">
         <f>S5</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G1" s="40"/>
       <c r="H1" s="41">
@@ -53928,7 +53928,7 @@
       </c>
       <c r="I1" s="41">
         <f>U5</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J1" s="14"/>
       <c r="M1" s="31" t="s">
@@ -53965,11 +53965,11 @@
       </c>
       <c r="E2" s="32" t="str">
         <f>"x DIV "&amp;E1</f>
-        <v>x DIV 5</v>
+        <v>x DIV 10</v>
       </c>
       <c r="F2" s="33" t="str">
         <f>"ax"&amp;E1</f>
-        <v>ax5</v>
+        <v>ax10</v>
       </c>
       <c r="G2" s="27" t="s">
         <v>3</v>
@@ -53988,19 +53988,19 @@
       </c>
       <c r="M2" s="30">
         <f>B1</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="N2" s="30">
         <f>C1</f>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="O2" s="30">
         <f>E1</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P2" s="30">
         <f>F1</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q2" s="30">
         <f>H1</f>
@@ -54008,7 +54008,7 @@
       </c>
       <c r="R2" s="30">
         <f>I1</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -54021,11 +54021,11 @@
       </c>
       <c r="C3" s="2">
         <f>C$1</f>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D3" s="25">
         <f>SUM(B3:C3)</f>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="E3" s="29">
         <f t="shared" ref="E3:E53" si="0">QUOTIENT(A3,$E$1)</f>
@@ -54037,7 +54037,7 @@
       </c>
       <c r="G3" s="4">
         <f>D3+F3</f>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="H3" s="5">
         <f>H$1</f>
@@ -54045,7 +54045,7 @@
       </c>
       <c r="I3" s="5">
         <f>I$1</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J3" s="15">
         <f>MIN(MAX(H3,INT(G3)),I3)</f>
@@ -54059,15 +54059,15 @@
       </c>
       <c r="B4" s="24">
         <f t="shared" ref="B4:B53" si="1">$B$1*A4</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:C53" si="2">C$1</f>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D4" s="25">
         <f t="shared" ref="D4:D53" si="3">SUM(B4:C4)</f>
-        <v>-13</v>
+        <v>10.5</v>
       </c>
       <c r="E4" s="29">
         <f t="shared" si="0"/>
@@ -54079,7 +54079,7 @@
       </c>
       <c r="G4" s="4">
         <f t="shared" ref="G4:G53" si="5">D4+F4</f>
-        <v>-13</v>
+        <v>10.5</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" ref="H4:I41" si="6">H$1</f>
@@ -54087,7 +54087,7 @@
       </c>
       <c r="I4" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J4" s="15">
         <f t="shared" ref="J4:J53" si="7">MIN(MAX(H4,INT(G4)),I4)</f>
@@ -54131,15 +54131,15 @@
       </c>
       <c r="B5" s="24">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D5" s="25">
         <f t="shared" si="3"/>
-        <v>-10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="29">
         <f t="shared" si="0"/>
@@ -54151,7 +54151,7 @@
       </c>
       <c r="G5" s="4">
         <f t="shared" si="5"/>
-        <v>-10</v>
+        <v>11</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="6"/>
@@ -54159,14 +54159,14 @@
       </c>
       <c r="I5" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J5" s="15">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="M5" s="42" t="s">
         <v>32</v>
@@ -54180,28 +54180,22 @@
         <v>Level</v>
       </c>
       <c r="P5">
-        <f>SUMIFS(Data!E:E,Data!$A:$A,'Reverser from Data'!$L5,Data!$B:$B,'Reverser from Data'!$M5)</f>
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="Q5">
-        <f>SUMIFS(Data!F:F,Data!$A:$A,'Reverser from Data'!$L5,Data!$B:$B,'Reverser from Data'!$M5)</f>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="R5">
-        <f>SUMIFS(Data!G:G,Data!$A:$A,'Reverser from Data'!$L5,Data!$B:$B,'Reverser from Data'!$M5)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S5">
-        <f>SUMIFS(Data!H:H,Data!$A:$A,'Reverser from Data'!$L5,Data!$B:$B,'Reverser from Data'!$M5)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T5">
-        <f>SUMIFS(Data!I:I,Data!$A:$A,'Reverser from Data'!$L5,Data!$B:$B,'Reverser from Data'!$M5)</f>
         <v>10</v>
       </c>
       <c r="U5">
-        <f>SUMIFS(Data!J:J,Data!$A:$A,'Reverser from Data'!$L5,Data!$B:$B,'Reverser from Data'!$M5)</f>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -54211,15 +54205,15 @@
       </c>
       <c r="B6" s="24">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D6" s="25">
         <f t="shared" si="3"/>
-        <v>-7</v>
+        <v>11.5</v>
       </c>
       <c r="E6" s="29">
         <f t="shared" si="0"/>
@@ -54231,7 +54225,7 @@
       </c>
       <c r="G6" s="4">
         <f t="shared" si="5"/>
-        <v>-7</v>
+        <v>11.5</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="6"/>
@@ -54239,14 +54233,14 @@
       </c>
       <c r="I6" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J6" s="15">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="M6" s="42" t="s">
         <v>36</v>
@@ -54261,27 +54255,27 @@
       </c>
       <c r="P6">
         <f>SUMIFS(Data!E:E,Data!$A:$A,'Reverser from Data'!$L6,Data!$B:$B,'Reverser from Data'!$M6)</f>
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="Q6">
         <f>SUMIFS(Data!F:F,Data!$A:$A,'Reverser from Data'!$L6,Data!$B:$B,'Reverser from Data'!$M6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <f>SUMIFS(Data!G:G,Data!$A:$A,'Reverser from Data'!$L6,Data!$B:$B,'Reverser from Data'!$M6)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="S6">
         <f>SUMIFS(Data!H:H,Data!$A:$A,'Reverser from Data'!$L6,Data!$B:$B,'Reverser from Data'!$M6)</f>
-        <v>-20</v>
+        <v>0.1</v>
       </c>
       <c r="T6">
         <f>SUMIFS(Data!I:I,Data!$A:$A,'Reverser from Data'!$L6,Data!$B:$B,'Reverser from Data'!$M6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6">
         <f>SUMIFS(Data!J:J,Data!$A:$A,'Reverser from Data'!$L6,Data!$B:$B,'Reverser from Data'!$M6)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -54291,15 +54285,15 @@
       </c>
       <c r="B7" s="24">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D7" s="25">
         <f t="shared" si="3"/>
-        <v>-4</v>
+        <v>12</v>
       </c>
       <c r="E7" s="29">
         <f t="shared" si="0"/>
@@ -54311,7 +54305,7 @@
       </c>
       <c r="G7" s="4">
         <f t="shared" si="5"/>
-        <v>-4</v>
+        <v>12</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="6"/>
@@ -54319,11 +54313,11 @@
       </c>
       <c r="I7" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J7" s="15">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="M7" s="42" t="s">
         <v>32</v>
@@ -54336,27 +54330,27 @@
       </c>
       <c r="B8" s="24">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>2.5</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D8" s="25">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>12.5</v>
       </c>
       <c r="E8" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
         <f t="shared" si="5"/>
-        <v>-0.5</v>
+        <v>12.5</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="6"/>
@@ -54364,11 +54358,11 @@
       </c>
       <c r="I8" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J8" s="15">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -54378,27 +54372,27 @@
       </c>
       <c r="B9" s="24">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D9" s="25">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E9" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="5"/>
-        <v>2.5</v>
+        <v>13</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="6"/>
@@ -54406,11 +54400,11 @@
       </c>
       <c r="I9" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J9" s="15">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -54420,27 +54414,27 @@
       </c>
       <c r="B10" s="24">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>3.5</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D10" s="25">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>13.5</v>
       </c>
       <c r="E10" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G10" s="4">
         <f t="shared" si="5"/>
-        <v>5.5</v>
+        <v>13.5</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="6"/>
@@ -54448,11 +54442,11 @@
       </c>
       <c r="I10" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J10" s="15">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -54462,27 +54456,27 @@
       </c>
       <c r="B11" s="24">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D11" s="25">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E11" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="5"/>
-        <v>8.5</v>
+        <v>14</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="6"/>
@@ -54490,11 +54484,11 @@
       </c>
       <c r="I11" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J11" s="15">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -54504,27 +54498,27 @@
       </c>
       <c r="B12" s="24">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>4.5</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D12" s="25">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>14.5</v>
       </c>
       <c r="E12" s="29">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G12" s="4">
         <f t="shared" si="5"/>
-        <v>11.5</v>
+        <v>14.5</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="6"/>
@@ -54532,11 +54526,11 @@
       </c>
       <c r="I12" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J12" s="15">
         <f t="shared" si="7"/>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -54546,19 +54540,19 @@
       </c>
       <c r="B13" s="24">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D13" s="25">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E13" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="4"/>
@@ -54566,7 +54560,7 @@
       </c>
       <c r="G13" s="4">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="6"/>
@@ -54574,11 +54568,11 @@
       </c>
       <c r="I13" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J13" s="15">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -54588,19 +54582,19 @@
       </c>
       <c r="B14" s="24">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>5.5</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D14" s="25">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>15.5</v>
       </c>
       <c r="E14" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="4"/>
@@ -54608,7 +54602,7 @@
       </c>
       <c r="G14" s="4">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>16.5</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="6"/>
@@ -54616,11 +54610,11 @@
       </c>
       <c r="I14" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J14" s="15">
         <f t="shared" si="7"/>
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -54630,19 +54624,19 @@
       </c>
       <c r="B15" s="24">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D15" s="25">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E15" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="4"/>
@@ -54650,7 +54644,7 @@
       </c>
       <c r="G15" s="4">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="6"/>
@@ -54658,11 +54652,11 @@
       </c>
       <c r="I15" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J15" s="15">
         <f t="shared" si="7"/>
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -54672,19 +54666,19 @@
       </c>
       <c r="B16" s="24">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>6.5</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D16" s="25">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>16.5</v>
       </c>
       <c r="E16" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="4"/>
@@ -54692,7 +54686,7 @@
       </c>
       <c r="G16" s="4">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>17.5</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="6"/>
@@ -54700,11 +54694,11 @@
       </c>
       <c r="I16" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J16" s="15">
         <f t="shared" si="7"/>
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -54714,19 +54708,19 @@
       </c>
       <c r="B17" s="24">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D17" s="25">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E17" s="29">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="4"/>
@@ -54734,7 +54728,7 @@
       </c>
       <c r="G17" s="4">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H17" s="5">
         <f t="shared" si="6"/>
@@ -54742,11 +54736,11 @@
       </c>
       <c r="I17" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J17" s="15">
         <f t="shared" si="7"/>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -54756,27 +54750,27 @@
       </c>
       <c r="B18" s="24">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>7.5</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D18" s="25">
         <f t="shared" si="3"/>
-        <v>29</v>
+        <v>17.5</v>
       </c>
       <c r="E18" s="29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G18" s="4">
         <f t="shared" si="5"/>
-        <v>30.5</v>
+        <v>18.5</v>
       </c>
       <c r="H18" s="5">
         <f t="shared" si="6"/>
@@ -54784,11 +54778,11 @@
       </c>
       <c r="I18" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J18" s="15">
         <f t="shared" si="7"/>
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -54798,27 +54792,27 @@
       </c>
       <c r="B19" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D19" s="25">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E19" s="29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="5"/>
-        <v>33.5</v>
+        <v>19</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="6"/>
@@ -54826,11 +54820,11 @@
       </c>
       <c r="I19" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J19" s="15">
         <f t="shared" si="7"/>
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -54840,27 +54834,27 @@
       </c>
       <c r="B20" s="24">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>8.5</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D20" s="25">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>18.5</v>
       </c>
       <c r="E20" s="29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="5"/>
-        <v>36.5</v>
+        <v>19.5</v>
       </c>
       <c r="H20" s="5">
         <f t="shared" si="6"/>
@@ -54868,11 +54862,11 @@
       </c>
       <c r="I20" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J20" s="15">
         <f t="shared" si="7"/>
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -54882,27 +54876,27 @@
       </c>
       <c r="B21" s="24">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D21" s="25">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="E21" s="29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="5"/>
-        <v>39.5</v>
+        <v>20</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="6"/>
@@ -54910,11 +54904,11 @@
       </c>
       <c r="I21" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J21" s="15">
         <f t="shared" si="7"/>
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -54924,27 +54918,27 @@
       </c>
       <c r="B22" s="24">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>9.5</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D22" s="25">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>19.5</v>
       </c>
       <c r="E22" s="29">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="5"/>
-        <v>42.5</v>
+        <v>20.5</v>
       </c>
       <c r="H22" s="5">
         <f t="shared" si="6"/>
@@ -54952,11 +54946,11 @@
       </c>
       <c r="I22" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J22" s="15">
         <f t="shared" si="7"/>
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -54966,19 +54960,19 @@
       </c>
       <c r="B23" s="24">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D23" s="25">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E23" s="29">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="4"/>
@@ -54986,7 +54980,7 @@
       </c>
       <c r="G23" s="4">
         <f t="shared" si="5"/>
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="H23" s="5">
         <f t="shared" si="6"/>
@@ -54994,11 +54988,11 @@
       </c>
       <c r="I23" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J23" s="15">
         <f t="shared" si="7"/>
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -55008,19 +55002,19 @@
       </c>
       <c r="B24" s="24">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>10.5</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D24" s="25">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>20.5</v>
       </c>
       <c r="E24" s="29">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="4"/>
@@ -55028,7 +55022,7 @@
       </c>
       <c r="G24" s="4">
         <f t="shared" si="5"/>
-        <v>49</v>
+        <v>22.5</v>
       </c>
       <c r="H24" s="5">
         <f t="shared" si="6"/>
@@ -55036,11 +55030,11 @@
       </c>
       <c r="I24" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J24" s="15">
         <f t="shared" si="7"/>
-        <v>49</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -55050,19 +55044,19 @@
       </c>
       <c r="B25" s="24">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D25" s="25">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E25" s="29">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="4"/>
@@ -55070,7 +55064,7 @@
       </c>
       <c r="G25" s="4">
         <f t="shared" si="5"/>
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="H25" s="5">
         <f t="shared" si="6"/>
@@ -55078,11 +55072,11 @@
       </c>
       <c r="I25" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J25" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -55092,19 +55086,19 @@
       </c>
       <c r="B26" s="24">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>11.5</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D26" s="25">
         <f t="shared" si="3"/>
-        <v>53</v>
+        <v>21.5</v>
       </c>
       <c r="E26" s="29">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="4"/>
@@ -55112,7 +55106,7 @@
       </c>
       <c r="G26" s="4">
         <f t="shared" si="5"/>
-        <v>55</v>
+        <v>23.5</v>
       </c>
       <c r="H26" s="5">
         <f t="shared" si="6"/>
@@ -55120,11 +55114,11 @@
       </c>
       <c r="I26" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J26" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -55134,19 +55128,19 @@
       </c>
       <c r="B27" s="24">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D27" s="25">
         <f t="shared" si="3"/>
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="E27" s="29">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="4"/>
@@ -55154,7 +55148,7 @@
       </c>
       <c r="G27" s="4">
         <f t="shared" si="5"/>
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="H27" s="5">
         <f t="shared" si="6"/>
@@ -55162,11 +55156,11 @@
       </c>
       <c r="I27" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J27" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -55176,27 +55170,27 @@
       </c>
       <c r="B28" s="24">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>12.5</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D28" s="25">
         <f t="shared" si="3"/>
-        <v>59</v>
+        <v>22.5</v>
       </c>
       <c r="E28" s="29">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="5"/>
-        <v>61.5</v>
+        <v>24.5</v>
       </c>
       <c r="H28" s="5">
         <f t="shared" si="6"/>
@@ -55204,11 +55198,11 @@
       </c>
       <c r="I28" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J28" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -55218,27 +55212,27 @@
       </c>
       <c r="B29" s="24">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D29" s="25">
         <f t="shared" si="3"/>
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E29" s="29">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="5"/>
-        <v>64.5</v>
+        <v>25</v>
       </c>
       <c r="H29" s="5">
         <f t="shared" si="6"/>
@@ -55246,11 +55240,11 @@
       </c>
       <c r="I29" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J29" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -55260,27 +55254,27 @@
       </c>
       <c r="B30" s="24">
         <f t="shared" si="1"/>
-        <v>81</v>
+        <v>13.5</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D30" s="25">
         <f t="shared" si="3"/>
-        <v>65</v>
+        <v>23.5</v>
       </c>
       <c r="E30" s="29">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="5"/>
-        <v>67.5</v>
+        <v>25.5</v>
       </c>
       <c r="H30" s="5">
         <f t="shared" si="6"/>
@@ -55288,11 +55282,11 @@
       </c>
       <c r="I30" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J30" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -55302,27 +55296,27 @@
       </c>
       <c r="B31" s="24">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="C31" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D31" s="25">
         <f t="shared" si="3"/>
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="E31" s="29">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="5"/>
-        <v>70.5</v>
+        <v>26</v>
       </c>
       <c r="H31" s="5">
         <f t="shared" si="6"/>
@@ -55330,11 +55324,11 @@
       </c>
       <c r="I31" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J31" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -55344,27 +55338,27 @@
       </c>
       <c r="B32" s="24">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>14.5</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D32" s="25">
         <f t="shared" si="3"/>
-        <v>71</v>
+        <v>24.5</v>
       </c>
       <c r="E32" s="29">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="G32" s="4">
         <f t="shared" si="5"/>
-        <v>73.5</v>
+        <v>26.5</v>
       </c>
       <c r="H32" s="5">
         <f t="shared" si="6"/>
@@ -55372,11 +55366,11 @@
       </c>
       <c r="I32" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J32" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -55386,19 +55380,19 @@
       </c>
       <c r="B33" s="24">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="C33" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D33" s="25">
         <f t="shared" si="3"/>
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="E33" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" si="4"/>
@@ -55406,7 +55400,7 @@
       </c>
       <c r="G33" s="4">
         <f t="shared" si="5"/>
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="H33" s="5">
         <f t="shared" si="6"/>
@@ -55414,11 +55408,11 @@
       </c>
       <c r="I33" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J33" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -55428,19 +55422,19 @@
       </c>
       <c r="B34" s="24">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>15.5</v>
       </c>
       <c r="C34" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D34" s="25">
         <f t="shared" si="3"/>
-        <v>77</v>
+        <v>25.5</v>
       </c>
       <c r="E34" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" si="4"/>
@@ -55448,7 +55442,7 @@
       </c>
       <c r="G34" s="4">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>28.5</v>
       </c>
       <c r="H34" s="5">
         <f t="shared" si="6"/>
@@ -55456,11 +55450,11 @@
       </c>
       <c r="I34" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J34" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -55470,19 +55464,19 @@
       </c>
       <c r="B35" s="24">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="C35" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D35" s="25">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="E35" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="4"/>
@@ -55490,7 +55484,7 @@
       </c>
       <c r="G35" s="4">
         <f t="shared" si="5"/>
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="H35" s="5">
         <f t="shared" si="6"/>
@@ -55498,11 +55492,11 @@
       </c>
       <c r="I35" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J35" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -55512,19 +55506,19 @@
       </c>
       <c r="B36" s="24">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>16.5</v>
       </c>
       <c r="C36" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D36" s="25">
         <f t="shared" si="3"/>
-        <v>83</v>
+        <v>26.5</v>
       </c>
       <c r="E36" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="4"/>
@@ -55532,7 +55526,7 @@
       </c>
       <c r="G36" s="4">
         <f t="shared" si="5"/>
-        <v>86</v>
+        <v>29.5</v>
       </c>
       <c r="H36" s="5">
         <f t="shared" si="6"/>
@@ -55540,11 +55534,11 @@
       </c>
       <c r="I36" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J36" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -55554,19 +55548,19 @@
       </c>
       <c r="B37" s="24">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="C37" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D37" s="25">
         <f t="shared" si="3"/>
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="E37" s="29">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="4"/>
@@ -55574,7 +55568,7 @@
       </c>
       <c r="G37" s="4">
         <f t="shared" si="5"/>
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="H37" s="5">
         <f t="shared" si="6"/>
@@ -55582,11 +55576,11 @@
       </c>
       <c r="I37" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J37" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -55596,27 +55590,27 @@
       </c>
       <c r="B38" s="24">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>17.5</v>
       </c>
       <c r="C38" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D38" s="25">
         <f t="shared" si="3"/>
-        <v>89</v>
+        <v>27.5</v>
       </c>
       <c r="E38" s="29">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" si="4"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G38" s="4">
         <f t="shared" si="5"/>
-        <v>92.5</v>
+        <v>30.5</v>
       </c>
       <c r="H38" s="5">
         <f t="shared" si="6"/>
@@ -55624,11 +55618,11 @@
       </c>
       <c r="I38" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J38" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -55638,27 +55632,27 @@
       </c>
       <c r="B39" s="24">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>18</v>
       </c>
       <c r="C39" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D39" s="25">
         <f t="shared" si="3"/>
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="E39" s="29">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F39" s="3">
         <f t="shared" si="4"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G39" s="4">
         <f t="shared" si="5"/>
-        <v>95.5</v>
+        <v>31</v>
       </c>
       <c r="H39" s="5">
         <f t="shared" si="6"/>
@@ -55666,11 +55660,11 @@
       </c>
       <c r="I39" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J39" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -55680,27 +55674,27 @@
       </c>
       <c r="B40" s="24">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>18.5</v>
       </c>
       <c r="C40" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D40" s="25">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>28.5</v>
       </c>
       <c r="E40" s="29">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F40" s="3">
         <f t="shared" si="4"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G40" s="4">
         <f t="shared" si="5"/>
-        <v>98.5</v>
+        <v>31.5</v>
       </c>
       <c r="H40" s="5">
         <f t="shared" si="6"/>
@@ -55708,11 +55702,11 @@
       </c>
       <c r="I40" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J40" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -55722,27 +55716,27 @@
       </c>
       <c r="B41" s="24">
         <f t="shared" si="1"/>
-        <v>114</v>
+        <v>19</v>
       </c>
       <c r="C41" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D41" s="25">
         <f t="shared" si="3"/>
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="E41" s="29">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F41" s="3">
         <f t="shared" si="4"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G41" s="4">
         <f t="shared" si="5"/>
-        <v>101.5</v>
+        <v>32</v>
       </c>
       <c r="H41" s="5">
         <f t="shared" si="6"/>
@@ -55750,11 +55744,11 @@
       </c>
       <c r="I41" s="5">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J41" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -55764,27 +55758,27 @@
       </c>
       <c r="B42" s="24">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>19.5</v>
       </c>
       <c r="C42" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D42" s="25">
         <f t="shared" si="3"/>
-        <v>101</v>
+        <v>29.5</v>
       </c>
       <c r="E42" s="29">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F42" s="3">
         <f t="shared" si="4"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="G42" s="4">
         <f t="shared" si="5"/>
-        <v>104.5</v>
+        <v>32.5</v>
       </c>
       <c r="H42" s="5">
         <f t="shared" ref="H42:I53" si="9">H$1</f>
@@ -55792,11 +55786,11 @@
       </c>
       <c r="I42" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J42" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -55806,19 +55800,19 @@
       </c>
       <c r="B43" s="24">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="C43" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D43" s="25">
         <f t="shared" si="3"/>
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="E43" s="29">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F43" s="3">
         <f t="shared" si="4"/>
@@ -55826,7 +55820,7 @@
       </c>
       <c r="G43" s="4">
         <f t="shared" si="5"/>
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="H43" s="5">
         <f t="shared" si="9"/>
@@ -55834,11 +55828,11 @@
       </c>
       <c r="I43" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J43" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -55848,19 +55842,19 @@
       </c>
       <c r="B44" s="24">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>20.5</v>
       </c>
       <c r="C44" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D44" s="25">
         <f t="shared" si="3"/>
-        <v>107</v>
+        <v>30.5</v>
       </c>
       <c r="E44" s="29">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F44" s="3">
         <f t="shared" si="4"/>
@@ -55868,7 +55862,7 @@
       </c>
       <c r="G44" s="4">
         <f t="shared" si="5"/>
-        <v>111</v>
+        <v>34.5</v>
       </c>
       <c r="H44" s="5">
         <f t="shared" si="9"/>
@@ -55876,11 +55870,11 @@
       </c>
       <c r="I44" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J44" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -55890,19 +55884,19 @@
       </c>
       <c r="B45" s="24">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>21</v>
       </c>
       <c r="C45" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D45" s="25">
         <f t="shared" si="3"/>
-        <v>110</v>
+        <v>31</v>
       </c>
       <c r="E45" s="29">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F45" s="3">
         <f t="shared" si="4"/>
@@ -55910,7 +55904,7 @@
       </c>
       <c r="G45" s="4">
         <f t="shared" si="5"/>
-        <v>114</v>
+        <v>35</v>
       </c>
       <c r="H45" s="5">
         <f t="shared" si="9"/>
@@ -55918,11 +55912,11 @@
       </c>
       <c r="I45" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J45" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -55932,19 +55926,19 @@
       </c>
       <c r="B46" s="24">
         <f t="shared" si="1"/>
-        <v>129</v>
+        <v>21.5</v>
       </c>
       <c r="C46" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D46" s="25">
         <f t="shared" si="3"/>
-        <v>113</v>
+        <v>31.5</v>
       </c>
       <c r="E46" s="29">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F46" s="3">
         <f t="shared" si="4"/>
@@ -55952,7 +55946,7 @@
       </c>
       <c r="G46" s="4">
         <f t="shared" si="5"/>
-        <v>117</v>
+        <v>35.5</v>
       </c>
       <c r="H46" s="5">
         <f t="shared" si="9"/>
@@ -55960,11 +55954,11 @@
       </c>
       <c r="I46" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J46" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -55974,19 +55968,19 @@
       </c>
       <c r="B47" s="24">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>22</v>
       </c>
       <c r="C47" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D47" s="25">
         <f t="shared" si="3"/>
-        <v>116</v>
+        <v>32</v>
       </c>
       <c r="E47" s="29">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F47" s="3">
         <f t="shared" si="4"/>
@@ -55994,7 +55988,7 @@
       </c>
       <c r="G47" s="4">
         <f t="shared" si="5"/>
-        <v>120</v>
+        <v>36</v>
       </c>
       <c r="H47" s="5">
         <f t="shared" si="9"/>
@@ -56002,11 +55996,11 @@
       </c>
       <c r="I47" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J47" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -56016,27 +56010,27 @@
       </c>
       <c r="B48" s="24">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>22.5</v>
       </c>
       <c r="C48" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D48" s="25">
         <f t="shared" si="3"/>
-        <v>119</v>
+        <v>32.5</v>
       </c>
       <c r="E48" s="29">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F48" s="3">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="G48" s="4">
         <f t="shared" si="5"/>
-        <v>123.5</v>
+        <v>36.5</v>
       </c>
       <c r="H48" s="5">
         <f t="shared" si="9"/>
@@ -56044,11 +56038,11 @@
       </c>
       <c r="I48" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J48" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -56058,27 +56052,27 @@
       </c>
       <c r="B49" s="24">
         <f t="shared" si="1"/>
-        <v>138</v>
+        <v>23</v>
       </c>
       <c r="C49" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D49" s="25">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="E49" s="29">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F49" s="3">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="G49" s="4">
         <f t="shared" si="5"/>
-        <v>126.5</v>
+        <v>37</v>
       </c>
       <c r="H49" s="5">
         <f t="shared" si="9"/>
@@ -56086,11 +56080,11 @@
       </c>
       <c r="I49" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J49" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -56100,27 +56094,27 @@
       </c>
       <c r="B50" s="24">
         <f t="shared" si="1"/>
-        <v>141</v>
+        <v>23.5</v>
       </c>
       <c r="C50" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D50" s="25">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>33.5</v>
       </c>
       <c r="E50" s="29">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F50" s="3">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="G50" s="4">
         <f t="shared" si="5"/>
-        <v>129.5</v>
+        <v>37.5</v>
       </c>
       <c r="H50" s="5">
         <f t="shared" si="9"/>
@@ -56128,11 +56122,11 @@
       </c>
       <c r="I50" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J50" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -56142,27 +56136,27 @@
       </c>
       <c r="B51" s="24">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>24</v>
       </c>
       <c r="C51" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D51" s="25">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="E51" s="29">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F51" s="3">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="G51" s="4">
         <f t="shared" si="5"/>
-        <v>132.5</v>
+        <v>38</v>
       </c>
       <c r="H51" s="5">
         <f t="shared" si="9"/>
@@ -56170,11 +56164,11 @@
       </c>
       <c r="I51" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J51" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -56184,27 +56178,27 @@
       </c>
       <c r="B52" s="24">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>24.5</v>
       </c>
       <c r="C52" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D52" s="25">
         <f t="shared" si="3"/>
-        <v>131</v>
+        <v>34.5</v>
       </c>
       <c r="E52" s="29">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F52" s="3">
         <f t="shared" si="4"/>
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="G52" s="4">
         <f t="shared" si="5"/>
-        <v>135.5</v>
+        <v>38.5</v>
       </c>
       <c r="H52" s="5">
         <f t="shared" si="9"/>
@@ -56212,11 +56206,11 @@
       </c>
       <c r="I52" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J52" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -56226,19 +56220,19 @@
       </c>
       <c r="B53" s="24">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="C53" s="2">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>10</v>
       </c>
       <c r="D53" s="25">
         <f t="shared" si="3"/>
-        <v>134</v>
+        <v>35</v>
       </c>
       <c r="E53" s="29">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F53" s="3">
         <f t="shared" si="4"/>
@@ -56246,7 +56240,7 @@
       </c>
       <c r="G53" s="4">
         <f t="shared" si="5"/>
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="H53" s="5">
         <f t="shared" si="9"/>
@@ -56254,11 +56248,11 @@
       </c>
       <c r="I53" s="5">
         <f t="shared" si="9"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J53" s="15">
         <f t="shared" si="7"/>
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>